<commit_message>
add content in doc
</commit_message>
<xml_diff>
--- a/doc/DSG-time.xlsx
+++ b/doc/DSG-time.xlsx
@@ -71,7 +71,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,8 +80,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -95,8 +96,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -110,98 +119,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,17 +135,92 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -240,13 +233,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,61 +287,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,13 +311,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,25 +329,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -378,49 +407,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,6 +424,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -473,39 +490,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -531,153 +515,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -685,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -826,16 +819,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>18837</c:v>
+                  <c:v>359</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1084108</c:v>
+                  <c:v>820519</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1068600</c:v>
+                  <c:v>873243</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1495235</c:v>
+                  <c:v>821160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -899,16 +892,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>20270</c:v>
+                  <c:v>13509</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77238</c:v>
+                  <c:v>23376</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>242584</c:v>
+                  <c:v>97727</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>779214</c:v>
+                  <c:v>360088</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -972,16 +965,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>18104</c:v>
+                  <c:v>17401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>176738</c:v>
+                  <c:v>76930</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>490247</c:v>
+                  <c:v>355049</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1110058</c:v>
+                  <c:v>568034</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1349,16 +1342,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>29383</c:v>
+                  <c:v>15385</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1364374</c:v>
+                  <c:v>921292</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1294183</c:v>
+                  <c:v>920779</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1975746</c:v>
+                  <c:v>956023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1422,16 +1415,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>17810</c:v>
+                  <c:v>14644</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>136453</c:v>
+                  <c:v>30970</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>822525</c:v>
+                  <c:v>211628</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1532985</c:v>
+                  <c:v>419759</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1495,16 +1488,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>18104</c:v>
+                  <c:v>17401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>176738</c:v>
+                  <c:v>76930</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>490247</c:v>
+                  <c:v>355049</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1110058</c:v>
+                  <c:v>568034</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1881,16 +1874,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>79835</c:v>
+                  <c:v>13505</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1338732</c:v>
+                  <c:v>830021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1302435</c:v>
+                  <c:v>879543</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2112478</c:v>
+                  <c:v>864186</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1954,16 +1947,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>17915</c:v>
+                  <c:v>11829</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>252629</c:v>
+                  <c:v>43073</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1328643</c:v>
+                  <c:v>252605</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1576349</c:v>
+                  <c:v>469767</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2027,16 +2020,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>19252</c:v>
+                  <c:v>12255</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>740479</c:v>
+                  <c:v>195130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1355986</c:v>
+                  <c:v>408894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1633351</c:v>
+                  <c:v>548823</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4374,7 +4367,7 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -4396,13 +4389,13 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>18837</v>
+        <v>359</v>
       </c>
       <c r="C3">
-        <v>29383</v>
+        <v>15385</v>
       </c>
       <c r="D3">
-        <v>79835</v>
+        <v>13505</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -4413,13 +4406,13 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1084108</v>
+        <v>820519</v>
       </c>
       <c r="C4">
-        <v>1364374</v>
+        <v>921292</v>
       </c>
       <c r="D4">
-        <v>1338732</v>
+        <v>830021</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -4430,13 +4423,13 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1068600</v>
+        <v>873243</v>
       </c>
       <c r="C5">
-        <v>1294183</v>
+        <v>920779</v>
       </c>
       <c r="D5">
-        <v>1302435</v>
+        <v>879543</v>
       </c>
       <c r="E5">
         <v>6</v>
@@ -4447,13 +4440,13 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1495235</v>
+        <v>821160</v>
       </c>
       <c r="C6">
-        <v>1975746</v>
+        <v>956023</v>
       </c>
       <c r="D6">
-        <v>2112478</v>
+        <v>864186</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -4464,13 +4457,13 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>20270</v>
+        <v>13509</v>
       </c>
       <c r="C7">
-        <v>17810</v>
+        <v>14644</v>
       </c>
       <c r="D7">
-        <v>17915</v>
+        <v>11829</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4478,13 +4471,13 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>77238</v>
+        <v>23376</v>
       </c>
       <c r="C8">
-        <v>136453</v>
+        <v>30970</v>
       </c>
       <c r="D8">
-        <v>252629</v>
+        <v>43073</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4492,13 +4485,13 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>242584</v>
+        <v>97727</v>
       </c>
       <c r="C9">
-        <v>822525</v>
+        <v>211628</v>
       </c>
       <c r="D9">
-        <v>1328643</v>
+        <v>252605</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4506,13 +4499,13 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>779214</v>
+        <v>360088</v>
       </c>
       <c r="C10">
-        <v>1532985</v>
+        <v>419759</v>
       </c>
       <c r="D10">
-        <v>1576349</v>
+        <v>469767</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4520,13 +4513,13 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>18104</v>
+        <v>17401</v>
       </c>
       <c r="C11">
-        <v>19472</v>
+        <v>12591</v>
       </c>
       <c r="D11">
-        <v>19252</v>
+        <v>12255</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4534,13 +4527,13 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>176738</v>
+        <v>76930</v>
       </c>
       <c r="C12">
-        <v>435827</v>
+        <v>169661</v>
       </c>
       <c r="D12">
-        <v>740479</v>
+        <v>195130</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4548,13 +4541,13 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>490247</v>
+        <v>355049</v>
       </c>
       <c r="C13">
-        <v>1187342</v>
+        <v>442177</v>
       </c>
       <c r="D13">
-        <v>1355986</v>
+        <v>408894</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4562,13 +4555,13 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>1110058</v>
+        <v>568034</v>
       </c>
       <c r="C14">
-        <v>1566532</v>
+        <v>514431</v>
       </c>
       <c r="D14">
-        <v>1633351</v>
+        <v>548823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>